<commit_message>
Ahora la puntuacion depende de los comentarios de los usuarios
</commit_message>
<xml_diff>
--- a/Comments/Comentarios-Locos al Carbon.xlsx
+++ b/Comments/Comentarios-Locos al Carbon.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Autor</t>
   </si>
@@ -33,6 +33,21 @@
   </si>
   <si>
     <t>04/04/2023</t>
+  </si>
+  <si>
+    <t>Starjerez</t>
+  </si>
+  <si>
+    <t>Esta chido, hacen promociones todos los meses</t>
+  </si>
+  <si>
+    <t>18/05/2023</t>
+  </si>
+  <si>
+    <t>Ta weno veri gud</t>
+  </si>
+  <si>
+    <t>SUper deli esta buenisimo ( No soy oriana)</t>
   </si>
 </sst>
 </file>
@@ -77,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -111,6 +126,48 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>